<commit_message>
changed ipad sample to run on simulator
1. selenium_action module updated selenium to 3.141.559
2.changed udid to auto to launch simulator to run the sample ipad tests
</commit_message>
<xml_diff>
--- a/example_usage/suites/sampleipadtest.xlsx
+++ b/example_usage/suites/sampleipadtest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mlin6/Documents/projects/2WorkSpace3Codeless/01GitHub/codeless/example_usage/suites/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C215BC95-AFC4-F845-AD81-28AB6DD8BA8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C65ABD-B57B-FF41-A7A5-9591B0CEC775}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ipad" sheetId="2" r:id="rId1"/>
@@ -229,9 +229,6 @@
     <t>assertEquals::WebElement::getText::Alert Views</t>
   </si>
   <si>
-    <t>6cc0740d415bc04c943707b6da5ac978c60c4fc2</t>
-  </si>
-  <si>
     <t>Click on the APP</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>UICatalog.catalog.alertviewTitle</t>
+  </si>
+  <si>
+    <t>auto</t>
   </si>
 </sst>
 </file>
@@ -627,7 +627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -858,7 +858,7 @@
         <v>55</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -874,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:G7"/>
     </sheetView>
   </sheetViews>
@@ -968,13 +968,13 @@
     </row>
     <row r="6" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
@@ -990,7 +990,7 @@
         <v>56</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">

</xml_diff>